<commit_message>
preparing data for RDA using exact dates
</commit_message>
<xml_diff>
--- a/data/dataRDA.xlsx
+++ b/data/dataRDA.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B127"/>
+  <dimension ref="A1:B208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,7 +360,7 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>ocsed</t>
+          <t>OC sed. rate (g C m-2 d-1)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -370,1514 +370,2027 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1.290298404</t>
-        </is>
+      <c r="A2">
+        <v>2.688575306375953</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BP 4 2006</t>
+          <t>BP 2006-04-20</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>0.565059239</t>
-        </is>
+      <c r="A3">
+        <v>1.290298404325461</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BP 5 2006</t>
+          <t>BP 2006-05-18</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1.182969964</t>
-        </is>
+      <c r="A4">
+        <v>0.565059238884132</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BP 6 2006</t>
+          <t>BP 2006-06-15</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>0.450401479</t>
-        </is>
+      <c r="A5">
+        <v>1.182969964232435</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BP 7 2006</t>
+          <t>BP 2006-07-13</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>0.948368788</t>
-        </is>
+      <c r="A6">
+        <v>0.450401478850263</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BP 8 2006</t>
+          <t>BP 2006-08-10</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>0.652827301</t>
-        </is>
+      <c r="A7">
+        <v>0.9483687881535803</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BP 9 2006</t>
+          <t>BP 2006-09-07</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>0.985265643</t>
-        </is>
+      <c r="A8">
+        <v>0.652827301160921</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BP 10 2006</t>
+          <t>BP 2006-10-05</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>0.453936626</t>
-        </is>
+      <c r="A9">
+        <v>0.9852656433525708</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BP 11 2006</t>
+          <t>BP 2006-11-02</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>0.572356326</t>
-        </is>
+      <c r="A10">
+        <v>0.4539366264064691</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BP 11 2006</t>
+          <t>BP 2006-11-30</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>1.229316547</t>
-        </is>
+      <c r="A11">
+        <v>0.5723563264878916</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>BP 12 2006</t>
+          <t>BP 2006-12-20</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>0.384157917</t>
-        </is>
+      <c r="A12">
+        <v>1.229316547382426</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BP 1 2007</t>
+          <t>BP 2007-01-24</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>0.814363309</t>
-        </is>
+      <c r="A13">
+        <v>0.384157917484542</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>BP 2 2007</t>
+          <t>BP 2007-02-15</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>1.340722369</t>
-        </is>
+      <c r="A14">
+        <v>0.8143633086936769</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BP 3 2007</t>
+          <t>BP 2007-03-15</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>1.490761563</t>
-        </is>
+      <c r="A15">
+        <v>1.340722368723062</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BP 4 2007</t>
+          <t>BP 2007-04-19</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2.500533381</t>
-        </is>
+      <c r="A16">
+        <v>1.490761563271751</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BP 5 2007</t>
+          <t>BP 2007-05-17</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2.469189805</t>
-        </is>
+      <c r="A17">
+        <v>2.500533381128984</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BP 6 2007</t>
+          <t>BP 2007-06-14</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>1.674978864</t>
-        </is>
+      <c r="A18">
+        <v>2.469189805153133</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BP 8 2007</t>
+          <t>BP 2007-07-16</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>1.341031595</t>
-        </is>
+      <c r="A19">
+        <v>0</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BP 9 2007</t>
+          <t>BP 2007-08-08</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>0.548375355</t>
-        </is>
+      <c r="A20">
+        <v>1.674978864449344</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BP 10 2007</t>
+          <t>BP 2007-09-11</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>0.856617894</t>
-        </is>
+      <c r="A21">
+        <v>1.341031595267631</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BP 11 2007</t>
+          <t>BP 2007-10-15</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>0.682936758</t>
-        </is>
+      <c r="A22">
+        <v>0.5483753549092405</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BP 12 2007</t>
+          <t>BP 2007-11-15</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>0.613236386</t>
-        </is>
+      <c r="A23">
+        <v>0.8566178936040352</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BP 1 2008</t>
+          <t>BP 2007-12-13</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>1.24649431</t>
-        </is>
+      <c r="A24">
+        <v>0.6829367577917972</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BP 2 2008</t>
+          <t>BP 2008-01-17</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>0.705239374</t>
-        </is>
+      <c r="A25">
+        <v>0.6132363861737116</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BP 3 2008</t>
+          <t>BP 2008-02-19</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>0.836825127</t>
-        </is>
+      <c r="A26">
+        <v>1.246494310336729</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BP 4 2008</t>
+          <t>BP 2008-03-18</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>0.637666238</t>
-        </is>
+      <c r="A27">
+        <v>0.7052393739971836</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>BP 5 2008</t>
+          <t>BP 2008-04-21</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>2.69778762</t>
-        </is>
+      <c r="A28">
+        <v>0.8368251267639946</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>BP 6 2008</t>
+          <t>BP 2008-05-18</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>1.763676181</t>
-        </is>
+      <c r="A29">
+        <v>0.6376662381956849</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BP 7 2008</t>
+          <t>BP 2008-06-18</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>1.455668094</t>
-        </is>
+      <c r="A30">
+        <v>2.697787620489218</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BP 8 2008</t>
+          <t>BP 2008-07-17</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>0.947285986</t>
-        </is>
+      <c r="A31">
+        <v>1.763676181463455</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>BP 9 2008</t>
+          <t>BP 2008-08-13</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>0.443096514</t>
-        </is>
+      <c r="A32">
+        <v>1.455668094176134</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>BP 10 2008</t>
+          <t>BP 2008-09-16</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>0.501916573</t>
-        </is>
+      <c r="A33">
+        <v>0.9472859859441302</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>BP 11 2008</t>
+          <t>BP 2008-10-16</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>0.300968162</t>
-        </is>
+      <c r="A34">
+        <v>0.4430965143606049</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>BP 12 2008</t>
+          <t>BP 2008-11-12</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>1.7</t>
-        </is>
+      <c r="A35">
+        <v>0.5019165733779709</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>CN 4 2006</t>
+          <t>BP 2008-12-17</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>1.6</t>
-        </is>
+      <c r="A36">
+        <v>0.8676745422283362</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>CN 6 2006</t>
+          <t>CH 2006-04-20</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A37">
+        <v>0.9650850287610718</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>CN 7 2006</t>
+          <t>CH 2006-05-18</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>2.8</t>
-        </is>
+      <c r="A38">
+        <v>0.9688102254129514</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>CN 10 2006</t>
+          <t>CH 2006-06-15</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
+      <c r="A39">
+        <v>0.4275533329951381</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>CN 11 2006</t>
+          <t>CH 2006-07-13</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>0.8</t>
-        </is>
+      <c r="A40">
+        <v>0.2835292930278588</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>CN 12 2006</t>
+          <t>CH 2006-08-10</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>1.8</t>
-        </is>
+      <c r="A41">
+        <v>0.9395899477137341</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>CN 12 2006</t>
+          <t>CH 2006-09-07</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>0.9</t>
-        </is>
+      <c r="A42">
+        <v>1.1228526761231</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>CN 1 2007</t>
+          <t>CH 2006-10-05</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>0.8</t>
-        </is>
+      <c r="A43">
+        <v>1.235562508728095</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>CN 3 2007</t>
+          <t>CH 2006-11-02</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A44">
+        <v>0.487781507197898</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>CN 4 2007</t>
+          <t>CH 2006-11-30</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>2.5</t>
-        </is>
+      <c r="A45">
+        <v>0.5109639681026237</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>CN 6 2007</t>
+          <t>CH 2006-12-20</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>1.1</t>
-        </is>
+      <c r="A46">
+        <v>0.4493465312245711</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>CN 7 2007</t>
+          <t>CH 2007-01-24</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>1.3</t>
-        </is>
+      <c r="A47">
+        <v>0.2992024970848352</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>CN 8 2007</t>
+          <t>CH 2007-02-15</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>0.4</t>
-        </is>
+      <c r="A48">
+        <v>0.4453298251427393</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>CN 10 2007</t>
+          <t>CH 2007-03-15</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>0.3</t>
-        </is>
+      <c r="A49">
+        <v>0.3166256961528646</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>CN 1 2008</t>
+          <t>CH 2007-04-19</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>0.8</t>
-        </is>
+      <c r="A50">
+        <v>0.3072065135102279</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>CN 2 2008</t>
+          <t>CH 2007-05-17</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
+      <c r="A51">
+        <v>0.5802186155108154</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>CN 3 2008</t>
+          <t>CH 2007-06-14</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>0.9</t>
-        </is>
+      <c r="A52">
+        <v>0.7508263996293815</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>CN 4 2008</t>
+          <t>CH 2007-07-16</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>0.8</t>
-        </is>
+      <c r="A53">
+        <v>0.3584704731451751</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>CN 5 2008</t>
+          <t>CH 2007-08-08</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>0.7</t>
-        </is>
+      <c r="A54">
+        <v>0.5756072347744663</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>CN 6 2008</t>
+          <t>CH 2007-09-11</t>
         </is>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>1.4</t>
-        </is>
+      <c r="A55">
+        <v>0.4047510682935785</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>CN 7 2008</t>
+          <t>CH 2007-10-15</t>
         </is>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>1.6</t>
-        </is>
+      <c r="A56">
+        <v>0.4088872459775869</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>CN 8 2008</t>
+          <t>CH 2007-11-15</t>
         </is>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>1.1</t>
-        </is>
-      </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>CN 9 2008</t>
+          <t>CH 2007-12-13</t>
         </is>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>2.5</t>
-        </is>
+      <c r="A58">
+        <v>0.3363508592967231</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>CN 10 2008</t>
+          <t>CH 2008-01-17</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>0.4</t>
-        </is>
+      <c r="A59">
+        <v>0.3116142092305593</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>CN 11 2008</t>
+          <t>CH 2008-02-19</t>
         </is>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>0.4</t>
-        </is>
+      <c r="A60">
+        <v>0.3094438575727165</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>CN 12 2008</t>
+          <t>CH 2008-03-18</t>
         </is>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>1.01815879</t>
-        </is>
+      <c r="A61">
+        <v>0.5465720595497054</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>MP 4 2006</t>
+          <t>CH 2008-04-21</t>
         </is>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>0.863026163</t>
-        </is>
+      <c r="A62">
+        <v>0.8740735602427021</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>MP 5 2006</t>
+          <t>CH 2008-05-18</t>
         </is>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>1.26120732</t>
-        </is>
+      <c r="A63">
+        <v>1.823537970515548</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>MP 6 2006</t>
+          <t>CH 2008-06-18</t>
         </is>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>1.38416877</t>
-        </is>
+      <c r="A64">
+        <v>0.3174974289659631</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>MP 7 2006</t>
+          <t>CH 2008-07-17</t>
         </is>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>0.966526011</t>
-        </is>
+      <c r="A65">
+        <v>1.343798283597439</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>MP 8 2006</t>
+          <t>CH 2008-08-13</t>
         </is>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>1.200894786</t>
-        </is>
+      <c r="A66">
+        <v>0.3572865717793633</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>MP 9 2006</t>
+          <t>CH 2008-09-16</t>
         </is>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>0.96779981</t>
-        </is>
+      <c r="A67">
+        <v>0.1970005981555252</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>MP 10 2006</t>
+          <t>CH 2008-10-16</t>
         </is>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>0.568331221</t>
-        </is>
+      <c r="A68">
+        <v>0.487938830135734</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>MP 11 2006</t>
+          <t>CH 2008-11-12</t>
         </is>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>0.740519741</t>
-        </is>
+      <c r="A69">
+        <v>0.2396201840378647</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>MP 11 2006</t>
+          <t>CH 2008-12-17</t>
         </is>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>1.543186295</t>
-        </is>
-      </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>MP 12 2006</t>
+          <t>CL 2006-04-20</t>
         </is>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>0.64665833</t>
-        </is>
+      <c r="A71">
+        <v>0.3089709592869438</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>MP 1 2007</t>
+          <t>CL 2006-05-18</t>
         </is>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>0.980310197</t>
-        </is>
-      </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>MP 2 2007</t>
+          <t>CL 2006-06-15</t>
         </is>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>1.263462298</t>
-        </is>
+      <c r="A73">
+        <v>0.7228475274523902</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>MP 3 2007</t>
+          <t>CL 2006-07-13</t>
         </is>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>0.891811882</t>
-        </is>
+      <c r="A74">
+        <v>0.7766926238374335</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>MP 4 2007</t>
+          <t>CL 2006-08-10</t>
         </is>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>1.737414401</t>
-        </is>
+      <c r="A75">
+        <v>2.794199081183045</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>MP 5 2007</t>
+          <t>CL 2006-09-07</t>
         </is>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>3.167867197</t>
-        </is>
+      <c r="A76">
+        <v>0.8224609896677724</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>MP 6 2007</t>
+          <t>CL 2006-10-05</t>
         </is>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>2.38763291</t>
-        </is>
+      <c r="A77">
+        <v>0.6481716534104246</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>MP 7 2007</t>
+          <t>CL 2006-11-02</t>
         </is>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>1.677331274</t>
-        </is>
+      <c r="A78">
+        <v>0.1699104092711298</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>MP 8 2007</t>
+          <t>CL 2006-11-30</t>
         </is>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>1.543195893</t>
-        </is>
+      <c r="A79">
+        <v>0.417144922642849</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>MP 9 2007</t>
+          <t>CL 2006-12-20</t>
         </is>
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>0.586173535</t>
-        </is>
+      <c r="A80">
+        <v>0.3621477361131641</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>MP 10 2007</t>
+          <t>CL 2007-01-24</t>
         </is>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>1.045637834</t>
-        </is>
+      <c r="A81">
+        <v>0.1087175183345706</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>MP 11 2007</t>
+          <t>CL 2007-02-15</t>
         </is>
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>0.935018412</t>
-        </is>
+      <c r="A82">
+        <v>0.2618402469779296</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>MP 12 2007</t>
+          <t>CL 2007-03-15</t>
         </is>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>0.917131896</t>
-        </is>
+      <c r="A83">
+        <v>0</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>MP 2 2008</t>
+          <t>CL 2007-04-19</t>
         </is>
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>0.506605248</t>
-        </is>
+      <c r="A84">
+        <v>0.4162213333289095</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>MP 3 2008</t>
+          <t>CL 2007-05-17</t>
         </is>
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>1.161853176</t>
-        </is>
+      <c r="A85">
+        <v>0.5531979364896982</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>MP 4 2008</t>
+          <t>CL 2007-06-14</t>
         </is>
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>0.433511922</t>
-        </is>
+      <c r="A86">
+        <v>0.6654975905008113</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>MP 5 2008</t>
+          <t>CL 2007-07-16</t>
         </is>
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>1.271276336</t>
-        </is>
+      <c r="A87">
+        <v>0.6847886452025094</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>MP 6 2008</t>
+          <t>CL 2007-08-08</t>
         </is>
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>1.828394109</t>
-        </is>
+      <c r="A88">
+        <v>0.6760060535772842</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>MP 7 2008</t>
+          <t>CL 2007-09-11</t>
         </is>
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>3.155419193</t>
-        </is>
+      <c r="A89">
+        <v>0.7818226742927524</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>MP 8 2008</t>
+          <t>CL 2007-10-15</t>
         </is>
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>4.347983122</t>
-        </is>
+      <c r="A90">
+        <v>0.3986115782456648</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>MP 9 2008</t>
+          <t>CL 2007-11-15</t>
         </is>
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>0.135402276</t>
-        </is>
-      </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>MP 10 2008</t>
+          <t>CL 2007-12-13</t>
         </is>
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>0.417410921</t>
-        </is>
+      <c r="A92">
+        <v>0.3280093516798149</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>MP 11 2008</t>
+          <t>CL 2008-01-17</t>
         </is>
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>0.4706145</t>
-        </is>
+      <c r="A93">
+        <v>0.1003502517787603</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>MP 12 2008</t>
+          <t>CL 2008-02-19</t>
         </is>
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>0.624872656</t>
-        </is>
+      <c r="A94">
+        <v>0.2228256897315996</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>TP 4 2006</t>
+          <t>CL 2008-03-18</t>
         </is>
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>0.72449926</t>
-        </is>
+      <c r="A95">
+        <v>0.5878571309508501</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>TP 5 2006</t>
+          <t>CL 2008-04-21</t>
         </is>
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>2.360171674</t>
-        </is>
+      <c r="A96">
+        <v>0.867387918620392</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>TP 6 2006</t>
+          <t>CL 2008-05-18</t>
         </is>
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>2.04109674</t>
-        </is>
+      <c r="A97">
+        <v>0.2083888359082883</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>TP 7 2006</t>
+          <t>CL 2008-06-18</t>
         </is>
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>2.032673281</t>
-        </is>
+      <c r="A98">
+        <v>0.2867308265216408</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>TP 8 2006</t>
+          <t>CL 2008-07-17</t>
         </is>
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>3.103888444</t>
-        </is>
+      <c r="A99">
+        <v>0.3598046752207302</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>TP 9 2006</t>
+          <t>CL 2008-08-13</t>
         </is>
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>2.604881138</t>
-        </is>
+      <c r="A100">
+        <v>0.2610733673258096</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>TP 10 2006</t>
+          <t>CL 2008-09-16</t>
         </is>
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>0.910621638</t>
-        </is>
+      <c r="A101">
+        <v>0.2547801278167355</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>TP 11 2006</t>
+          <t>CL 2008-10-16</t>
         </is>
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>0.7939045</t>
-        </is>
+      <c r="A102">
+        <v>0.2839979734662801</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>TP 11 2006</t>
+          <t>CL 2008-11-12</t>
         </is>
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>0.132368419</t>
-        </is>
+      <c r="A103">
+        <v>0.4528614007773957</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>TP 12 2006</t>
+          <t>CL 2008-12-17</t>
         </is>
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>1.022812979</t>
-        </is>
-      </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>TP 1 2007</t>
+          <t>CN 2006-04-20</t>
         </is>
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>1.128691847</t>
-        </is>
+      <c r="A105">
+        <v>1.720836635785624</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>TP 2 2007</t>
+          <t>CN 2006-05-18</t>
         </is>
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>0.76894927</t>
-        </is>
-      </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>TP 3 2007</t>
+          <t>CN 2006-06-15</t>
         </is>
       </c>
     </row>
     <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>0.699166476</t>
-        </is>
+      <c r="A107">
+        <v>1.609517221748461</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>TP 4 2007</t>
+          <t>CN 2006-07-13</t>
         </is>
       </c>
     </row>
     <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>2.059790855</t>
-        </is>
+      <c r="A108">
+        <v>2.031219467135676</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>TP 5 2007</t>
+          <t>CN 2006-08-10</t>
         </is>
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>4.320374136</t>
-        </is>
-      </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>TP 6 2007</t>
+          <t>CN 2006-09-07</t>
         </is>
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>1.31424253</t>
-        </is>
-      </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>TP 7 2007</t>
+          <t>CN 2006-10-05</t>
         </is>
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>3.414799156</t>
-        </is>
-      </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>TP 8 2007</t>
+          <t>CN 2006-10-15</t>
         </is>
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>1.774920078</t>
-        </is>
+      <c r="A112">
+        <v>2.785158678642631</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>TP 9 2007</t>
+          <t>CN 2006-11-02</t>
         </is>
       </c>
     </row>
     <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>0.810656759</t>
-        </is>
+      <c r="A113">
+        <v>0.537303763108351</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>TP 10 2007</t>
+          <t>CN 2006-11-30</t>
         </is>
       </c>
     </row>
     <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>0.45691095</t>
-        </is>
+      <c r="A114">
+        <v>0.7526382581934651</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>TP 11 2007</t>
+          <t>CN 2006-12-20</t>
         </is>
       </c>
     </row>
     <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>0.421763179</t>
-        </is>
+      <c r="A115">
+        <v>1.832269829643075</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>TP 12 2007</t>
+          <t>CN 2007-01-24</t>
         </is>
       </c>
     </row>
     <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>0.535959707</t>
-        </is>
+      <c r="A116">
+        <v>0.9415266289472181</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>TP 1 2008</t>
+          <t>CN 2007-02-15</t>
         </is>
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>0.330240305</t>
-        </is>
-      </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>TP 2 2008</t>
+          <t>CN 2007-03-15</t>
         </is>
       </c>
     </row>
     <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>1.479569106</t>
-        </is>
+      <c r="A118">
+        <v>0.7926668003066853</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>TP 3 2008</t>
+          <t>CN 2007-04-19</t>
         </is>
       </c>
     </row>
     <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>1.060414095</t>
-        </is>
+      <c r="A119">
+        <v>1.973085358781913</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>TP 4 2008</t>
+          <t>CN 2007-05-17</t>
         </is>
       </c>
     </row>
     <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>0.292314599</t>
-        </is>
-      </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>TP 5 2008</t>
+          <t>CN 2007-06-14</t>
         </is>
       </c>
     </row>
     <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>2.338888847</t>
-        </is>
+      <c r="A121">
+        <v>2.480105045493279</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>TP 6 2008</t>
+          <t>CN 2007-07-16</t>
         </is>
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>1.929643676</t>
-        </is>
+      <c r="A122">
+        <v>1.081423176949782</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>TP 7 2008</t>
+          <t>CN 2007-08-08</t>
         </is>
       </c>
     </row>
     <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>2.93853881</t>
-        </is>
+      <c r="A123">
+        <v>1.292891743919795</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>TP 8 2008</t>
+          <t>CN 2007-09-11</t>
         </is>
       </c>
     </row>
     <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>12.22341174</t>
-        </is>
-      </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>TP 9 2008</t>
+          <t>CN 2007-10-15</t>
         </is>
       </c>
     </row>
     <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>1.021109732</t>
-        </is>
+      <c r="A125">
+        <v>0.4092561130939449</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>TP 10 2008</t>
+          <t>CN 2007-11-15</t>
         </is>
       </c>
     </row>
     <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>0.326229967</t>
-        </is>
-      </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>TP 11 2008</t>
+          <t>CN 2007-12-13</t>
         </is>
       </c>
     </row>
     <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>0.342410998</t>
-        </is>
-      </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>TP 12 2008</t>
+          <t>CN 2008-01-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128">
+        <v>0.3124697787424062</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>CN 2008-02-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129">
+        <v>0.7726789403592991</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>CN 2008-03-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130">
+        <v>0.5419398452155872</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>CN 2008-04-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131">
+        <v>0.9170495619085425</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>CN 2008-05-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132">
+        <v>0.7926050016294992</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>CN 2008-06-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133">
+        <v>0.701302897851947</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>CN 2008-07-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134">
+        <v>1.415657756502862</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>CN 2008-08-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135">
+        <v>1.633151620560684</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>CN 2008-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>NA 2008-09-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137">
+        <v>1.118145695677462</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>CN 2008-10-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138">
+        <v>2.543451668640317</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>CN 2008-11-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139">
+        <v>0.3761741746214576</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>CN 2008-12-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140">
+        <v>0.403693276623143</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>MP 2006-04-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141">
+        <v>1.018158789743072</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>MP 2006-05-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142">
+        <v>0.8630261626453746</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>MP 2006-06-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143">
+        <v>1.261207319857927</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>MP 2006-07-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144">
+        <v>1.384168769858198</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>MP 2006-08-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145">
+        <v>0.9665260110924309</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>MP 2006-09-07</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146">
+        <v>1.200894786175743</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>MP 2006-10-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147">
+        <v>0.9677998102676965</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>MP 2006-11-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148">
+        <v>0.5683312211864912</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>MP 2006-11-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149">
+        <v>0.7405197411432577</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>MP 2006-12-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150">
+        <v>1.54318629524265</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>MP 2007-01-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151">
+        <v>0.646658330197027</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>MP 2007-02-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152">
+        <v>0.9803101974346955</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>MP 2007-03-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153">
+        <v>1.263462297524134</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>MP 2007-04-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154">
+        <v>0.8918118824676219</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>MP 2007-05-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155">
+        <v>1.737414400981016</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>MP 2007-06-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156">
+        <v>3.167867196769605</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>MP 2007-07-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157">
+        <v>2.387632909796011</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>MP 2007-08-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158">
+        <v>1.67733127395628</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>MP 2007-09-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159">
+        <v>1.543195893062574</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>MP 2007-10-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160">
+        <v>0.5861735346867899</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>MP 2007-11-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161">
+        <v>1.045637834416685</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>MP 2007-12-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162">
+        <v>0.9350184123954335</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>MP 2008-01-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163">
+        <v>0</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>MP 2008-02-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164">
+        <v>0.9171318964827426</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>MP 2008-03-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165">
+        <v>0.5066052475762431</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>MP 2008-04-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166">
+        <v>1.16185317615386</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>MP 2008-05-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167">
+        <v>0.4335119215765796</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>MP 2008-06-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168">
+        <v>1.271276336318565</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>MP 2008-07-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169">
+        <v>1.828394109300967</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>MP 2008-08-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170">
+        <v>3.155419193266736</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>MP 2008-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171">
+        <v>4.347983122130319</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>MP 2008-10-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172">
+        <v>0.1354022763788915</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>MP 2008-11-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173">
+        <v>0.4174109209872516</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>MP 2008-12-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174">
+        <v>1.026768763180631</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>TP 2006-04-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175">
+        <v>0.6248726559015475</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>TP 2006-05-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176">
+        <v>0.7244992601486647</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>TP 2006-06-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177">
+        <v>2.360171674088278</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>TP 2006-07-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178">
+        <v>2.041096739795821</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>TP 2006-08-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179">
+        <v>2.032673281242595</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>TP 2006-09-07</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180">
+        <v>3.103888443845911</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>TP 2006-10-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181">
+        <v>2.604881137844109</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>TP 2006-11-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182">
+        <v>0.9106216375507346</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>TP 2006-11-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183">
+        <v>0.7939045002889128</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>TP 2006-12-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184">
+        <v>0.132368418796195</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>TP 2007-01-24</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185">
+        <v>1.022812978728179</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>TP 2007-02-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186">
+        <v>1.128691846732926</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>TP 2007-03-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187">
+        <v>0.7689492704068163</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>TP 2007-04-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188">
+        <v>0.6991664763679767</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>TP 2007-05-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189">
+        <v>2.059790854636199</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>TP 2007-06-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190">
+        <v>4.320374135535593</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>TP 2007-07-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191">
+        <v>1.314242529909834</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>TP 2007-08-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192">
+        <v>3.414799156045417</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>TP 2007-09-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193">
+        <v>1.774920078154649</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>TP 2007-10-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194">
+        <v>0.8106567594447419</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>TP 2007-11-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195">
+        <v>0.4569109503118013</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>TP 2007-12-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196">
+        <v>0.4217631786644312</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>TP 2008-01-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197">
+        <v>0.5359597070045018</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>TP 2008-02-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198">
+        <v>0.3302403045363838</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>TP 2008-03-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199">
+        <v>1.479569106462002</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>TP 2008-04-21</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200">
+        <v>1.060414095130752</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>TP 2008-05-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201">
+        <v>0.2923145991815035</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>TP 2008-06-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202">
+        <v>0.3035936374090192</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>TP 2008-06-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203">
+        <v>2.338888847358537</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>TP 2008-07-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204">
+        <v>1.929643675593499</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>TP 2008-08-13</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205">
+        <v>2.938538810168837</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>TP 2008-09-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206">
+        <v>12.22341174370256</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>TP 2008-10-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207">
+        <v>1.021109732206891</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>TP 2008-11-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208">
+        <v>0.32622996678651</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>TP 2008-12-17</t>
         </is>
       </c>
     </row>

</xml_diff>